<commit_message>
Chi vua change duoc 1 huong
</commit_message>
<xml_diff>
--- a/ranks.xlsx
+++ b/ranks.xlsx
@@ -442,52 +442,52 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>23</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>12</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>10</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>8</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>7</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>5</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>4</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>3</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
open path thanh cong, nhung chua update duoc hinh anh moi buoc di chuyen
</commit_message>
<xml_diff>
--- a/ranks.xlsx
+++ b/ranks.xlsx
@@ -442,52 +442,52 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>126</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>96</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>92</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>90</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>89</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>83</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>78</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>77</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>64</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>23</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>